<commit_message>
Population and Ideal coverage
</commit_message>
<xml_diff>
--- a/data/population_hazard.xlsx
+++ b/data/population_hazard.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianesamson/Projects/riesgo-vis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5E3DEA76-58BE-C541-9F36-D0C2796398C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52552328-4E1A-104F-B327-5DA6052CF417}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16480"/>
+    <workbookView xWindow="5300" yWindow="-17140" windowWidth="28040" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="population_hazard" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>flood_hazard_level</t>
   </si>
@@ -59,11 +59,14 @@
   <si>
     <t>% increase</t>
   </si>
+  <si>
+    <t>covered by # of centers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -897,11 +900,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1087,6 +1090,59 @@
         <v>-8.3458385297244697E-2</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>123456.91</v>
+      </c>
+      <c r="C14">
+        <f>B14/SUM(B2:B5)</f>
+        <v>0.86623040549094132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>50806.17</v>
+      </c>
+      <c r="C15">
+        <f>B15/SUM(B2:B5)</f>
+        <v>0.35647943270685856</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>30096.84</v>
+      </c>
+      <c r="C16">
+        <f>B16/SUM(B2:B5)</f>
+        <v>0.21117325808005386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4484.16</v>
+      </c>
+      <c r="C17">
+        <f>B17/SUM(B2:B5)</f>
+        <v>3.1462926903696675E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>